<commit_message>
Seeding DB and Excel and vise-versa
</commit_message>
<xml_diff>
--- a/ADCBackEnd/ExcelData/courses.xlsx
+++ b/ADCBackEnd/ExcelData/courses.xlsx
@@ -13,28 +13,31 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>الاسم</t>
+    <t>اسم المادة</t>
   </si>
   <si>
-    <t>رقم العسكري</t>
+    <t>كود المادة</t>
   </si>
   <si>
-    <t>طالب11</t>
+    <t>القسم</t>
   </si>
   <si>
-    <t>1111</t>
+    <t>سنة دراسية</t>
   </si>
   <si>
-    <t>طالب222</t>
+    <t>Electronics</t>
   </si>
   <si>
-    <t>22222</t>
+    <t>ECE213</t>
   </si>
   <si>
-    <t>محمد</t>
+    <t>عام</t>
   </si>
   <si>
-    <t>1234</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>اتصالات</t>
   </si>
 </sst>
 </file>
@@ -92,13 +95,25 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -108,12 +123,10 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>